<commit_message>
Everything but non additive multipliers
</commit_message>
<xml_diff>
--- a/src/main/java/com/alchcalc/Ingredients.xlsx
+++ b/src/main/java/com/alchcalc/Ingredients.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Projects\alchcalc\src\main\java\com\alchcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302D6788-EC1E-401A-BA78-79135336139A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11753B-3F54-4F29-B676-FE720ADD8C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5EAA879D-E245-444B-B395-22AAE924D7EE}"/>
   </bookViews>
   <sheets>
     <sheet name="AllIngredients" sheetId="1" r:id="rId1"/>
+    <sheet name="AllIngredients (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AllIngredients!$A$1:$A$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AllIngredients (2)'!$A$1:$A$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
   <si>
     <t>DH</t>
   </si>
@@ -330,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -354,11 +356,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -679,6 +692,1063 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="29.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0.432</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C58" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C59" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C60" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C61" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A64" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G64">
+    <sortCondition descending="1" ref="E1:E64"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:G41 A43:G63 A42:C42 E42:G42 B2:B63">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB87681-4582-4390-B5EB-F1994A261996}">
+  <dimension ref="A1:G63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
@@ -1718,7 +2788,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A64" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}"/>
-  <conditionalFormatting sqref="A2:G41 A43:G63 A42:C42 E42:G42 B2:B63">
+  <conditionalFormatting sqref="A2:G41 A43:G63 A42:C42 E42:G42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixes, Not Accounting for Pure Multipliers
</commit_message>
<xml_diff>
--- a/src/main/java/com/alchcalc/Ingredients.xlsx
+++ b/src/main/java/com/alchcalc/Ingredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Projects\alchcalc\src\main\java\com\alchcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11753B-3F54-4F29-B676-FE720ADD8C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99C2D5D-1310-4202-9CDB-6142E937297E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5EAA879D-E245-444B-B395-22AAE924D7EE}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="9" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Fixing Adder And Multiplier Functions Before Musefruit Bug Fix
</commit_message>
<xml_diff>
--- a/src/main/java/com/alchcalc/Ingredients.xlsx
+++ b/src/main/java/com/alchcalc/Ingredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Projects\alchcalc\src\main\java\com\alchcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF12F78-ACC7-4522-B519-6FC5CC634685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0D8C7-AC49-4AA0-BDA3-6079DC94270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5EAA879D-E245-444B-B395-22AAE924D7EE}"/>
   </bookViews>
@@ -692,8 +692,8 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9" t="b">
         <v>0</v>
@@ -1091,7 +1091,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="9" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Cleaning up some logic
</commit_message>
<xml_diff>
--- a/src/main/java/com/alchcalc/Ingredients.xlsx
+++ b/src/main/java/com/alchcalc/Ingredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Projects\alchcalc\src\main\java\com\alchcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0D8C7-AC49-4AA0-BDA3-6079DC94270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964CE7B0-FB0C-4608-99AF-5E0AF0D1C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5EAA879D-E245-444B-B395-22AAE924D7EE}"/>
   </bookViews>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -356,10 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +690,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +728,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6" t="b">
         <v>0</v>
@@ -741,20 +738,20 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+        <v>0.21</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C3" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6">
@@ -765,7 +762,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="b">
         <v>0</v>
@@ -775,14 +772,14 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
-        <v>0.69</v>
+        <v>0.44</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="b">
         <v>0</v>
@@ -792,14 +789,14 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
-        <v>0.69</v>
+        <v>0.44</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="b">
         <v>0</v>
@@ -809,31 +806,29 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+        <v>0.44</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C7" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="b">
         <v>0</v>
@@ -842,15 +837,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9" s="6" t="b">
         <v>0</v>
@@ -867,24 +860,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="6" t="b">
         <v>0</v>
@@ -896,29 +887,29 @@
       <c r="E11" s="6">
         <v>0.69</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
-        <v>0.56000000000000005</v>
+        <v>0.21</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B13" s="6" t="b">
         <v>0</v>
@@ -927,15 +918,13 @@
         <v>1</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B14" s="6" t="b">
         <v>0</v>
@@ -944,21 +933,19 @@
         <v>1</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="6">
-        <v>0.56000000000000005</v>
-      </c>
+      <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
@@ -969,7 +956,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="b">
         <v>0</v>
@@ -979,48 +966,44 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+        <v>0.21</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B19" s="6" t="b">
         <v>0</v>
@@ -1030,48 +1013,46 @@
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+        <v>0.21</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B20" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C20" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6">
-        <v>0.44</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B21" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6" t="b">
         <v>0</v>
@@ -1080,25 +1061,21 @@
         <v>1</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="11">
-        <v>0.432</v>
-      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="6">
         <v>0.44</v>
       </c>
@@ -1107,7 +1084,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B24" s="6" t="b">
         <v>0</v>
@@ -1117,65 +1094,63 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
-        <v>0.44</v>
+        <v>0.21</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B25" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B26" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C26" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+        <v>0.69</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B27" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6">
-        <v>0.21</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+        <v>0.69</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B28" s="6" t="b">
         <v>0</v>
@@ -1185,14 +1160,14 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6">
-        <v>0.21</v>
+        <v>0.44</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B29" s="6" t="b">
         <v>0</v>
@@ -1202,14 +1177,14 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6">
-        <v>0.21</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B30" s="6" t="b">
         <v>0</v>
@@ -1219,14 +1194,14 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6">
-        <v>0.21</v>
+        <v>0.69</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B31" s="6" t="b">
         <v>0</v>
@@ -1235,9 +1210,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
@@ -1260,7 +1233,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B33" s="6" t="b">
         <v>0</v>
@@ -1270,33 +1243,31 @@
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6">
-        <v>0.21</v>
+        <v>0.69</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B34" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" s="6">
-        <v>2.4</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D34" s="6"/>
       <c r="E34" s="6">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+        <v>0.69</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B35" s="6" t="b">
         <v>0</v>
@@ -1311,22 +1282,24 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B36" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C36" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="E36" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B37" s="6" t="b">
         <v>0</v>
@@ -1341,7 +1314,7 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B38" s="6" t="b">
         <v>0</v>
@@ -1351,12 +1324,12 @@
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B39" s="6" t="b">
         <v>0</v>
@@ -1371,7 +1344,7 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B40" s="6" t="b">
         <v>0</v>
@@ -1380,13 +1353,15 @@
         <v>1</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="E40" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B41" s="6" t="b">
         <v>0</v>
@@ -1401,22 +1376,26 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B42" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="D42" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B43" s="6" t="b">
         <v>0</v>
@@ -1425,13 +1404,15 @@
         <v>1</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="E43" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44" s="6" t="b">
         <v>0</v>
@@ -1446,7 +1427,7 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B45" s="6" t="b">
         <v>0</v>
@@ -1461,7 +1442,7 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B46" s="6" t="b">
         <v>0</v>
@@ -1470,13 +1451,15 @@
         <v>1</v>
       </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B47" s="6" t="b">
         <v>0</v>
@@ -1485,19 +1468,21 @@
         <v>1</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B48" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C48" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -1506,7 +1491,7 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B49" s="6" t="b">
         <v>0</v>
@@ -1521,7 +1506,7 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B50" s="6" t="b">
         <v>0</v>
@@ -1536,7 +1521,7 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B51" s="6" t="b">
         <v>0</v>
@@ -1551,13 +1536,13 @@
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B52" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C52" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -1566,13 +1551,13 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B53" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C53" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -1581,7 +1566,7 @@
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B54" s="6" t="b">
         <v>0</v>
@@ -1596,7 +1581,7 @@
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B55" s="6" t="b">
         <v>0</v>
@@ -1611,7 +1596,7 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B56" s="6" t="b">
         <v>0</v>
@@ -1626,13 +1611,13 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B57" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C57" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -1641,37 +1626,43 @@
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B58" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
+      <c r="D58" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="B59" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C59" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
+      <c r="E59" s="6">
+        <v>0.96</v>
+      </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B60" s="6" t="b">
         <v>0</v>
@@ -1686,22 +1677,24 @@
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B61" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C61" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
+      <c r="E61" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B62" s="6" t="b">
         <v>0</v>
@@ -1710,13 +1703,15 @@
         <v>1</v>
       </c>
       <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
+      <c r="E62" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B63" s="6" t="b">
         <v>0</v>
@@ -1725,14 +1720,16 @@
         <v>1</v>
       </c>
       <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
+      <c r="E63" s="6">
+        <v>0.21</v>
+      </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A64" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G64">
-    <sortCondition descending="1" ref="E1:E64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G63">
+    <sortCondition ref="A1:A63"/>
   </sortState>
   <conditionalFormatting sqref="A2:G41 A43:G63 A42:C42 E42:G42 B2:B63">
     <cfRule type="expression" dxfId="1" priority="1">

</xml_diff>

<commit_message>
Fixing Concurrent Modification Exception
</commit_message>
<xml_diff>
--- a/src/main/java/com/alchcalc/Ingredients.xlsx
+++ b/src/main/java/com/alchcalc/Ingredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Projects\alchcalc\src\main\java\com\alchcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964CE7B0-FB0C-4608-99AF-5E0AF0D1C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BA7896-B210-4832-9F85-39690DD74902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5EAA879D-E245-444B-B395-22AAE924D7EE}"/>
   </bookViews>
@@ -689,8 +689,8 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +765,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="9" t="b">
         <v>1</v>
@@ -799,7 +799,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="9" t="b">
         <v>0</v>
@@ -927,7 +927,7 @@
         <v>38</v>
       </c>
       <c r="B14" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="9" t="b">
         <v>1</v>
@@ -942,7 +942,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="9" t="b">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="9" t="b">
         <v>0</v>
@@ -1070,7 +1070,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="9" t="b">
         <v>1</v>
@@ -1119,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="9" t="b">
         <v>0</v>
@@ -1153,7 +1153,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="9" t="b">
         <v>1</v>
@@ -1170,7 +1170,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="9" t="b">
         <v>1</v>
@@ -1285,7 +1285,7 @@
         <v>20</v>
       </c>
       <c r="B36" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="9" t="b">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>22</v>
       </c>
       <c r="B46" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="9" t="b">
         <v>1</v>
@@ -1462,7 +1462,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="9" t="b">
         <v>1</v>
@@ -1680,7 +1680,7 @@
         <v>23</v>
       </c>
       <c r="B61" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61" s="9" t="b">
         <v>0</v>
@@ -1697,7 +1697,7 @@
         <v>24</v>
       </c>
       <c r="B62" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62" s="9" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Changes Before Working out Adder/Healer Problem
</commit_message>
<xml_diff>
--- a/src/main/java/com/alchcalc/Ingredients.xlsx
+++ b/src/main/java/com/alchcalc/Ingredients.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\Projects\alchcalc\src\main\java\com\alchcalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BA7896-B210-4832-9F85-39690DD74902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC90DAB-FC5C-407C-B3CE-03890453C85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5EAA879D-E245-444B-B395-22AAE924D7EE}"/>
   </bookViews>
   <sheets>
     <sheet name="AllIngredients" sheetId="1" r:id="rId1"/>
-    <sheet name="AllIngredients (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Website Test" sheetId="6" r:id="rId2"/>
+    <sheet name="Discovery Ingredients" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AllIngredients!$A$1:$A$64</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AllIngredients (2)'!$A$1:$A$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Discovery Ingredients'!$A$1:$A$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Website Test'!$A$1:$A$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
   <si>
     <t>DH</t>
   </si>
@@ -119,9 +121,6 @@
     <t>Allium</t>
   </si>
   <si>
-    <t>Common Reedmace Shoots</t>
-  </si>
-  <si>
     <t>Elaiva Oil</t>
   </si>
   <si>
@@ -246,6 +245,36 @@
   </si>
   <si>
     <t>Guano</t>
+  </si>
+  <si>
+    <t>Negative Poison Multiplier?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karuva </t>
+  </si>
+  <si>
+    <t>Don't know what this does but it "multiplies something"</t>
+  </si>
+  <si>
+    <t>Nymph Herb</t>
+  </si>
+  <si>
+    <t>This might be BAD</t>
+  </si>
+  <si>
+    <t>Do these have Direct Healing?</t>
+  </si>
+  <si>
+    <t>Apparently has a great HoT (and some Direct Healing?)</t>
+  </si>
+  <si>
+    <t>Drakon</t>
+  </si>
+  <si>
+    <t>Not in game yet, has DH</t>
+  </si>
+  <si>
+    <t>Thymus</t>
   </si>
 </sst>
 </file>
@@ -332,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -349,7 +378,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -361,7 +389,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -686,54 +742,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="9" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
@@ -743,14 +799,14 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="6"/>
@@ -760,14 +816,14 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="b">
+      <c r="C4" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="6"/>
@@ -777,14 +833,14 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="b">
+      <c r="C5" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
@@ -794,14 +850,14 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="b">
+      <c r="C6" s="8" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="6"/>
@@ -811,44 +867,50 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="6"/>
@@ -858,14 +920,14 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="6"/>
@@ -873,14 +935,14 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C11" s="9" t="b">
+      <c r="C11" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="6"/>
@@ -889,32 +951,33 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="6"/>
@@ -922,116 +985,116 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B14" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="9" t="b">
-        <v>1</v>
+      <c r="C14" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="9" t="b">
-        <v>0</v>
+      <c r="C15" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.21</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>0.21</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
-        <v>0.21</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C20" s="9" t="b">
-        <v>0</v>
+      <c r="C20" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6">
-        <v>0.56000000000000005</v>
-      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
@@ -1040,9 +1103,9 @@
         <v>41</v>
       </c>
       <c r="B21" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="6"/>
@@ -1052,194 +1115,196 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B23" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="9" t="b">
+      <c r="C23" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+        <v>0.21</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B24" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="B25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="E25" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C26" s="9" t="b">
+      <c r="C26" s="8" t="b">
         <v>0</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <v>0.69</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B27" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6">
-        <v>0.69</v>
+        <v>0.44</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B28" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C28" s="9" t="b">
+      <c r="C28" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="B29" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+        <v>0.69</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B30" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C31" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6">
+        <v>0.21</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B32" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C32" s="9" t="b">
-        <v>0</v>
+      <c r="C32" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6">
-        <v>0.21</v>
+        <v>0.69</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B33" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C33" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6">
@@ -1250,50 +1315,48 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B34" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C34" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C34" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B35" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C35" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B36" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C36" s="9" t="b">
-        <v>0</v>
+      <c r="C36" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
@@ -1302,122 +1365,122 @@
         <v>44</v>
       </c>
       <c r="B37" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B39" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="E39" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B40" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B41" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C41" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="C41" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B42" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C42" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" s="11">
-        <v>0.3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C42" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="6"/>
       <c r="E42" s="6">
-        <v>0.44</v>
+        <v>0.69</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B43" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B44" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D44" s="6"/>
@@ -1427,76 +1490,76 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B45" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="E45" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B46" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C46" s="9" t="b">
+      <c r="C46" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6">
-        <v>0.44</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B47" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C47" s="9" t="b">
-        <v>1</v>
+      <c r="C47" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C48" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C48" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D49" s="6"/>
@@ -1511,23 +1574,27 @@
       <c r="B50" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C50" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="C50" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E50" s="6">
+        <v>0.21</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B51" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C51" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C51" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -1536,33 +1603,33 @@
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B52" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C52" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C52" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C53" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C53" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
@@ -1571,10 +1638,12 @@
       <c r="B54" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C54" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" s="6"/>
+      <c r="C54" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="6">
+        <v>3</v>
+      </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -1586,10 +1655,12 @@
       <c r="B55" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C55" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D55" s="6"/>
+      <c r="C55" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="6">
+        <v>4.2</v>
+      </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -1599,9 +1670,9 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D56" s="6"/>
@@ -1614,76 +1685,78 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="C57" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B58" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C58" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" s="6">
-        <v>2.4</v>
-      </c>
+      <c r="C58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" s="6"/>
       <c r="E58" s="6">
-        <v>0</v>
-      </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
+        <v>0.96</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="B59" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C59" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C59" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D59" s="6"/>
-      <c r="E59" s="6">
-        <v>0.96</v>
-      </c>
+      <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B60" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60" s="9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C60" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+      <c r="E60" s="6">
+        <v>0.44</v>
+      </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B61" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C61" s="9" t="b">
-        <v>0</v>
+      <c r="C61" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6">
@@ -1692,31 +1765,15 @@
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-    </row>
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C63" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C63" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D63" s="6"/>
@@ -1731,8 +1788,18 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G63">
     <sortCondition ref="A1:A63"/>
   </sortState>
-  <conditionalFormatting sqref="A2:G41 A43:G63 A42:C42 E42:G42 B2:B63">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A42:G49 A41:C41 E41:G41 A63:G63 A51:G61 A50:C50 F50:G50 A2:G40 B2:B61">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1742,18 +1809,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB87681-4582-4390-B5EB-F1994A261996}">
-  <dimension ref="A1:G63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8567D357-CE5B-40FA-A597-A80CFE678B48}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="9" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
@@ -1762,25 +1829,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1788,9 +1855,9 @@
         <v>25</v>
       </c>
       <c r="B2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
@@ -1802,30 +1869,30 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="b">
+      <c r="C3" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6">
-        <v>0.96</v>
+        <v>0.44</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6">
@@ -1836,46 +1903,42 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="b">
+      <c r="C5" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B6" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B7" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="9" t="b">
+      <c r="C7" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="6"/>
@@ -1885,44 +1948,495 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A27" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}"/>
+  <conditionalFormatting sqref="A16:C16 E16:G16 A17:G25 A2:G15 B2:B25">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA0AF1E-5568-42C3-9F4B-5750711678EE}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="29.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="B4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="B8" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="9" t="b">
+      <c r="C8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B9" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="9" t="b">
+      <c r="C9" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="6"/>
@@ -1932,46 +2446,42 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B11" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C11" s="9" t="b">
+      <c r="C11" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C12" s="9" t="b">
+      <c r="C12" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="6"/>
@@ -1981,12 +2491,12 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="6"/>
@@ -1996,61 +2506,57 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="9" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B16" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C16" s="9" t="b">
+      <c r="C16" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <v>0.21</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B17" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="9" t="b">
+      <c r="C17" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B18" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C18" s="9" t="b">
+      <c r="C18" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
@@ -2058,48 +2564,44 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B19" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C19" s="9" t="b">
+      <c r="C19" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="6"/>
@@ -2107,14 +2609,14 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="6"/>
@@ -2122,671 +2624,165 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B23" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C23" s="9" t="b">
+      <c r="C23" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B24" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C24" s="9" t="b">
-        <v>1</v>
+      <c r="C24" s="8" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B25" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C25" s="9" t="b">
+      <c r="C25" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="B26" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C26" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B27" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C27" s="9" t="b">
-        <v>0</v>
+      <c r="C27" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B28" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="6">
-        <v>0.44</v>
-      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B29" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8" t="b">
         <v>1</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30" s="9" t="b">
-        <v>1</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="6">
-        <v>0.69</v>
-      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9" t="b">
-        <v>1</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C32" s="9" t="b">
-        <v>0</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6">
-        <v>0.21</v>
-      </c>
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C34" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C36" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C42" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" s="8">
-        <v>0.432</v>
-      </c>
-      <c r="E42" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6">
-        <v>0.69</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C46" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C47" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C48" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C50" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C51" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B52" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C52" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C53" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C54" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C55" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C57" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C58" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C59" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B61" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C61" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B63" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C63" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6">
-        <v>0.21</v>
-      </c>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
+      <c r="H32" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A64" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}"/>
-  <conditionalFormatting sqref="A2:G41 A43:G63 A42:C42 E42:G42">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <autoFilter ref="A1:A33" xr:uid="{E8B70718-34BF-49C0-BD81-04B2CF484DC5}"/>
+  <conditionalFormatting sqref="A32:G32 A2:G28">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:G31">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>